<commit_message>
Refactor Helper and PerjalananDinas to utilize centralized akun_perjalanan array for improved maintainability and query efficiency
</commit_message>
<xml_diff>
--- a/storage/app/public/templates/BuyPo9w8pzuhPqE3t9QTzEt3yigtVNYC5O2ExHe5.xlsx
+++ b/storage/app/public/templates/BuyPo9w8pzuhPqE3t9QTzEt3yigtVNYC5O2ExHe5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhlis/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhlis/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C58D1F1-4C24-CD40-8AE3-CC98CE320866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D630B8-9BCD-714E-8292-991C789E0BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="3020" windowWidth="27640" windowHeight="16940" xr2:uid="{E6B8D688-EC68-9A41-86AB-CF45890BDB9C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>kode</t>
   </si>
@@ -45,547 +45,553 @@
     <t>wilayah</t>
   </si>
   <si>
-    <t>PANGAMBAU HILIR LUAR</t>
-  </si>
-  <si>
-    <t>PENGAMBAU HILIR DALAM</t>
-  </si>
-  <si>
-    <t>TABAT PADANG</t>
-  </si>
-  <si>
-    <t>LOKBUNTAR</t>
-  </si>
-  <si>
-    <t>PENGAMBAU HULU</t>
-  </si>
-  <si>
-    <t>SUNGAI HARANG</t>
-  </si>
-  <si>
-    <t>BATU PANGGUNG</t>
-  </si>
-  <si>
-    <t>HAPULANG</t>
-  </si>
-  <si>
-    <t>MANGUNANG</t>
-  </si>
-  <si>
-    <t>MANGUNANG SEBERANG</t>
-  </si>
-  <si>
-    <t>HARUYAN SEBERANG</t>
-  </si>
-  <si>
-    <t>HARUYAN</t>
-  </si>
-  <si>
-    <t>ANDANG</t>
-  </si>
-  <si>
-    <t>TELUK MESJID</t>
-  </si>
-  <si>
-    <t>BARIKIN</t>
-  </si>
-  <si>
-    <t>PANGGUNG</t>
-  </si>
-  <si>
-    <t>PANDANU</t>
-  </si>
-  <si>
-    <t>MURUNG A</t>
-  </si>
-  <si>
-    <t>PAGAT</t>
-  </si>
-  <si>
-    <t>HALIAU</t>
-  </si>
-  <si>
-    <t>BARU</t>
-  </si>
-  <si>
-    <t>ALUAN MATI</t>
-  </si>
-  <si>
-    <t>ALUAN SUMUR</t>
-  </si>
-  <si>
-    <t>KALI BARU</t>
-  </si>
-  <si>
-    <t>LAYUH</t>
-  </si>
-  <si>
-    <t>KAHAKAN</t>
-  </si>
-  <si>
-    <t>BAKTI</t>
-  </si>
-  <si>
-    <t>ALUAN BESAR</t>
-  </si>
-  <si>
-    <t>PAYA BESAR</t>
-  </si>
-  <si>
-    <t>PANTAI BATUNG</t>
-  </si>
-  <si>
-    <t>ALUAN</t>
-  </si>
-  <si>
-    <t>KINDINGAN</t>
-  </si>
-  <si>
-    <t>HARUYAN DAYAK</t>
-  </si>
-  <si>
-    <t>TILAHAN</t>
-  </si>
-  <si>
-    <t>PASTING</t>
-  </si>
-  <si>
-    <t>BATU TUNGGAL</t>
-  </si>
-  <si>
-    <t>BULAYAK</t>
-  </si>
-  <si>
-    <t>MURUNG B</t>
-  </si>
-  <si>
-    <t>DATAR AJAB</t>
-  </si>
-  <si>
-    <t>ALAT</t>
-  </si>
-  <si>
-    <t>HANTAKAN</t>
-  </si>
-  <si>
-    <t>HINAS KANAN</t>
-  </si>
-  <si>
-    <t>PATIKALAIN</t>
-  </si>
-  <si>
-    <t>TANAH HABANG</t>
-  </si>
-  <si>
-    <t>CUKAN LIPAI</t>
-  </si>
-  <si>
-    <t>PAYA</t>
-  </si>
-  <si>
-    <t>KIAS</t>
-  </si>
-  <si>
-    <t>KAPAR</t>
-  </si>
-  <si>
-    <t>TEMBUK BAHALANG</t>
-  </si>
-  <si>
-    <t>BANUA RANTAU</t>
-  </si>
-  <si>
-    <t>LOK BESAR</t>
-  </si>
-  <si>
-    <t>LUNJUK</t>
-  </si>
-  <si>
-    <t>BIRAYANG TIMUR</t>
-  </si>
-  <si>
-    <t>BIRAYANG</t>
-  </si>
-  <si>
-    <t>LIMBAR</t>
-  </si>
-  <si>
-    <t>MAHELA</t>
-  </si>
-  <si>
-    <t>BIRAYANG SURAPATI</t>
-  </si>
-  <si>
-    <t>WAWAI</t>
-  </si>
-  <si>
-    <t>WAWAI GARDU</t>
-  </si>
-  <si>
-    <t>ANDUHUM</t>
-  </si>
-  <si>
-    <t>LABUHAN</t>
-  </si>
-  <si>
-    <t>RANGAS</t>
-  </si>
-  <si>
-    <t>JUHU</t>
-  </si>
-  <si>
-    <t>HINAS KIRI</t>
-  </si>
-  <si>
-    <t>ATIRAN</t>
-  </si>
-  <si>
-    <t>MUARA HUNGI</t>
-  </si>
-  <si>
-    <t>PEMBAKULAN</t>
-  </si>
-  <si>
-    <t>NATEH</t>
-  </si>
-  <si>
-    <t>BATU TANGGA</t>
-  </si>
-  <si>
-    <t>TANDILANG</t>
-  </si>
-  <si>
-    <t>BATU PERAHU</t>
-  </si>
-  <si>
-    <t>AING BANTAI</t>
-  </si>
-  <si>
-    <t>DATAR BATUNG</t>
-  </si>
-  <si>
-    <t>PAJUKUNGAN</t>
-  </si>
-  <si>
-    <t>BUKAT</t>
-  </si>
-  <si>
-    <t>BARABAI BARAT</t>
-  </si>
-  <si>
-    <t>BARABAI UTARA</t>
-  </si>
-  <si>
-    <t>BARABAI SELATAN</t>
-  </si>
-  <si>
-    <t>BARABAI DARAT</t>
-  </si>
-  <si>
-    <t>BENAWA TENGAH</t>
-  </si>
-  <si>
-    <t>KAYU BAWANG</t>
-  </si>
-  <si>
-    <t>AWANG BESAR</t>
-  </si>
-  <si>
-    <t>GAMBAH</t>
-  </si>
-  <si>
-    <t>MANDINGIN</t>
-  </si>
-  <si>
-    <t>BARABAI TIMUR</t>
-  </si>
-  <si>
-    <t>BANUA BINJAI</t>
-  </si>
-  <si>
-    <t>BANUA BUDI</t>
-  </si>
-  <si>
-    <t>BABAI</t>
-  </si>
-  <si>
-    <t>BANUA JINGAH</t>
-  </si>
-  <si>
-    <t>BAKAPAS</t>
-  </si>
-  <si>
-    <t>AYUANG</t>
-  </si>
-  <si>
-    <t>PANGGANG MARAK</t>
-  </si>
-  <si>
-    <t>MUNDAR</t>
-  </si>
-  <si>
-    <t>TABUDARAT HILIR</t>
-  </si>
-  <si>
-    <t>MAHANG BARU</t>
-  </si>
-  <si>
-    <t>JAMIL</t>
-  </si>
-  <si>
-    <t>TABUDARAT HULU</t>
-  </si>
-  <si>
-    <t>PANTAI HAMBAWANG BARAT</t>
-  </si>
-  <si>
-    <t>PANTAI HAMBAWANG TIMUR</t>
-  </si>
-  <si>
-    <t>BENUA KEPAYANG</t>
-  </si>
-  <si>
-    <t>SUNGAI JARANIH</t>
-  </si>
-  <si>
-    <t>BATANG BAHALANG</t>
-  </si>
-  <si>
-    <t>TAAL</t>
-  </si>
-  <si>
-    <t>MURUNG TAAL</t>
-  </si>
-  <si>
-    <t>SUNGAI RANGAS</t>
-  </si>
-  <si>
-    <t>DURIAN GANTANG</t>
-  </si>
-  <si>
-    <t>GUHA</t>
-  </si>
-  <si>
-    <t>BANGKAL</t>
-  </si>
-  <si>
-    <t>TARAS PADANG</t>
-  </si>
-  <si>
-    <t>PAHALATAN</t>
-  </si>
-  <si>
-    <t>PERUMAHAN</t>
-  </si>
-  <si>
-    <t>KADUNDUNG</t>
-  </si>
-  <si>
-    <t>KASARANGAN</t>
-  </si>
-  <si>
-    <t>PEMANGKIH SEBERANG</t>
-  </si>
-  <si>
-    <t>TABAT</t>
-  </si>
-  <si>
-    <t>MANTAAS</t>
-  </si>
-  <si>
-    <t>RANTAU BUJUR</t>
-  </si>
-  <si>
-    <t>BINJAI PIRUA</t>
-  </si>
-  <si>
-    <t>BINJAI PEMANGKIH</t>
-  </si>
-  <si>
-    <t>TUNGKUP</t>
-  </si>
-  <si>
-    <t>PEMANGKIH</t>
-  </si>
-  <si>
-    <t>RANTAU KEMINTING</t>
-  </si>
-  <si>
-    <t>BANUA KUPANG</t>
-  </si>
-  <si>
-    <t>SUNGAI BULUH</t>
-  </si>
-  <si>
-    <t>SAMHURANG</t>
-  </si>
-  <si>
-    <t>MASIRAAN</t>
-  </si>
-  <si>
-    <t>JARANIH</t>
-  </si>
-  <si>
-    <t>BANUA HANYAR</t>
-  </si>
-  <si>
-    <t>BANUA ASAM</t>
-  </si>
-  <si>
-    <t>MATANG GINALUN</t>
-  </si>
-  <si>
-    <t>HULU RASAU</t>
-  </si>
-  <si>
-    <t>BANUA SUPANGGAL</t>
-  </si>
-  <si>
-    <t>MAHANG PUTAT</t>
-  </si>
-  <si>
-    <t>MAHANG SEI HANYAR</t>
-  </si>
-  <si>
-    <t>MAHANG MATANG LANDUNG</t>
-  </si>
-  <si>
-    <t>BULUAN</t>
-  </si>
-  <si>
-    <t>PANDAWAN</t>
-  </si>
-  <si>
-    <t>BANUA BATUNG</t>
-  </si>
-  <si>
-    <t>JATUH</t>
-  </si>
-  <si>
-    <t>HILIR BANUA</t>
-  </si>
-  <si>
-    <t>KAMBAT SELATAN</t>
-  </si>
-  <si>
-    <t>WALATUNG</t>
-  </si>
-  <si>
-    <t>KAYU RABAH</t>
-  </si>
-  <si>
-    <t>SETIAP</t>
-  </si>
-  <si>
-    <t>KAMBAT UTARA</t>
-  </si>
-  <si>
-    <t>PALAJAU</t>
-  </si>
-  <si>
-    <t>SUMANGGI</t>
-  </si>
-  <si>
-    <t>ILUNG PASAR LAMA</t>
-  </si>
-  <si>
-    <t>DANGU</t>
-  </si>
-  <si>
-    <t>HAPINGIN</t>
-  </si>
-  <si>
-    <t>ILUNG</t>
-  </si>
-  <si>
-    <t>ILUNG TENGAH</t>
-  </si>
-  <si>
-    <t>SUMANGGI SEBERANG</t>
-  </si>
-  <si>
-    <t>AWANG BARU</t>
-  </si>
-  <si>
-    <t>AWANG</t>
-  </si>
-  <si>
-    <t>MARINGGIT</t>
-  </si>
-  <si>
-    <t>LABUNGANAK</t>
-  </si>
-  <si>
-    <t>MUARA RINTIS</t>
-  </si>
-  <si>
-    <t>TELANG</t>
-  </si>
-  <si>
-    <t>HAUR GADING</t>
-  </si>
-  <si>
-    <t>LIMPASU</t>
-  </si>
-  <si>
-    <t>KABANG</t>
-  </si>
-  <si>
-    <t>TAPUK</t>
-  </si>
-  <si>
-    <t>PAUH</t>
-  </si>
-  <si>
-    <t>HAWANG</t>
-  </si>
-  <si>
-    <t>KARATUNGAN</t>
-  </si>
-  <si>
-    <t>ABUNG</t>
-  </si>
-  <si>
-    <t>ABUNG SURAPATI</t>
-  </si>
-  <si>
-    <t>KARAU</t>
-  </si>
-  <si>
-    <t>HULU SUNGAI TENGAH</t>
-  </si>
-  <si>
-    <t>KECAMATAN HARUYAN</t>
-  </si>
-  <si>
-    <t>KECAMATAN BATU BENAWA</t>
-  </si>
-  <si>
-    <t>KECAMATAN HANTAKAN</t>
-  </si>
-  <si>
-    <t>KECAMATAN BATANG ALAI SELATAN</t>
-  </si>
-  <si>
-    <t>KECAMATAN BATANG ALAI TIMUR</t>
-  </si>
-  <si>
-    <t>KECAMATAN BARABAI</t>
-  </si>
-  <si>
-    <t>KECAMATAN LABUAN AMAS SELATAN</t>
-  </si>
-  <si>
-    <t>KECAMATAN LABUAN AMAS UTARA</t>
-  </si>
-  <si>
-    <t>KECAMATAN PANDAWAN</t>
-  </si>
-  <si>
-    <t>KECAMATAN BATANG ALAI UTARA</t>
-  </si>
-  <si>
-    <t>KECAMATAN LIMPASU</t>
+    <t>Banjarbaru</t>
+  </si>
+  <si>
+    <t>Banjarmasin</t>
+  </si>
+  <si>
+    <t>Hulu Sungai Tengah</t>
+  </si>
+  <si>
+    <t>Kecamatan Haruyan</t>
+  </si>
+  <si>
+    <t>Kecamatan Batu Benawa</t>
+  </si>
+  <si>
+    <t>Kecamatan Hantakan</t>
+  </si>
+  <si>
+    <t>Kecamatan Batang Alai Selatan</t>
+  </si>
+  <si>
+    <t>Kecamatan Batang Alai Timur</t>
+  </si>
+  <si>
+    <t>Kecamatan Barabai</t>
+  </si>
+  <si>
+    <t>Kecamatan Labuan Amas Selatan</t>
+  </si>
+  <si>
+    <t>Kecamatan Labuan Amas Utara</t>
+  </si>
+  <si>
+    <t>Kecamatan Pandawan</t>
+  </si>
+  <si>
+    <t>Kecamatan Batang Alai Utara</t>
+  </si>
+  <si>
+    <t>Kecamatan Limpasu</t>
+  </si>
+  <si>
+    <t>Pangambau Hilir Luar</t>
+  </si>
+  <si>
+    <t>Pengambau Hilir Dalam</t>
+  </si>
+  <si>
+    <t>Tabat Padang</t>
+  </si>
+  <si>
+    <t>Lokbuntar</t>
+  </si>
+  <si>
+    <t>Pengambau Hulu</t>
+  </si>
+  <si>
+    <t>Sungai Harang</t>
+  </si>
+  <si>
+    <t>Batu Panggung</t>
+  </si>
+  <si>
+    <t>Hapulang</t>
+  </si>
+  <si>
+    <t>Mangunang</t>
+  </si>
+  <si>
+    <t>Mangunang Seberang</t>
+  </si>
+  <si>
+    <t>Haruyan Seberang</t>
+  </si>
+  <si>
+    <t>Haruyan</t>
+  </si>
+  <si>
+    <t>Andang</t>
+  </si>
+  <si>
+    <t>Teluk Mesjid</t>
+  </si>
+  <si>
+    <t>Barikin</t>
+  </si>
+  <si>
+    <t>Panggung</t>
+  </si>
+  <si>
+    <t>Pandanu</t>
+  </si>
+  <si>
+    <t>Murung A</t>
+  </si>
+  <si>
+    <t>Pagat</t>
+  </si>
+  <si>
+    <t>Haliau</t>
+  </si>
+  <si>
+    <t>Baru</t>
+  </si>
+  <si>
+    <t>Aluan Mati</t>
+  </si>
+  <si>
+    <t>Aluan Sumur</t>
+  </si>
+  <si>
+    <t>Kali Baru</t>
+  </si>
+  <si>
+    <t>Layuh</t>
+  </si>
+  <si>
+    <t>Kahakan</t>
+  </si>
+  <si>
+    <t>Bakti</t>
+  </si>
+  <si>
+    <t>Aluan Besar</t>
+  </si>
+  <si>
+    <t>Paya Besar</t>
+  </si>
+  <si>
+    <t>Pantai Batung</t>
+  </si>
+  <si>
+    <t>Aluan</t>
+  </si>
+  <si>
+    <t>Kindingan</t>
+  </si>
+  <si>
+    <t>Haruyan Dayak</t>
+  </si>
+  <si>
+    <t>Tilahan</t>
+  </si>
+  <si>
+    <t>Pasting</t>
+  </si>
+  <si>
+    <t>Batu Tunggal</t>
+  </si>
+  <si>
+    <t>Bulayak</t>
+  </si>
+  <si>
+    <t>Murung B</t>
+  </si>
+  <si>
+    <t>Datar Ajab</t>
+  </si>
+  <si>
+    <t>Alat</t>
+  </si>
+  <si>
+    <t>Hantakan</t>
+  </si>
+  <si>
+    <t>Hinas Kanan</t>
+  </si>
+  <si>
+    <t>Patikalain</t>
+  </si>
+  <si>
+    <t>Tanah Habang</t>
+  </si>
+  <si>
+    <t>Cukan Lipai</t>
+  </si>
+  <si>
+    <t>Paya</t>
+  </si>
+  <si>
+    <t>Kias</t>
+  </si>
+  <si>
+    <t>Kapar</t>
+  </si>
+  <si>
+    <t>Tembuk Bahalang</t>
+  </si>
+  <si>
+    <t>Banua Rantau</t>
+  </si>
+  <si>
+    <t>Lok Besar</t>
+  </si>
+  <si>
+    <t>Lunjuk</t>
+  </si>
+  <si>
+    <t>Birayang Timur</t>
+  </si>
+  <si>
+    <t>Birayang</t>
+  </si>
+  <si>
+    <t>Limbar</t>
+  </si>
+  <si>
+    <t>Mahela</t>
+  </si>
+  <si>
+    <t>Birayang Surapati</t>
+  </si>
+  <si>
+    <t>Wawai</t>
+  </si>
+  <si>
+    <t>Wawai Gardu</t>
+  </si>
+  <si>
+    <t>Anduhum</t>
+  </si>
+  <si>
+    <t>Labuhan</t>
+  </si>
+  <si>
+    <t>Rangas</t>
+  </si>
+  <si>
+    <t>Juhu</t>
+  </si>
+  <si>
+    <t>Hinas Kiri</t>
+  </si>
+  <si>
+    <t>Atiran</t>
+  </si>
+  <si>
+    <t>Muara Hungi</t>
+  </si>
+  <si>
+    <t>Pembakulan</t>
+  </si>
+  <si>
+    <t>Nateh</t>
+  </si>
+  <si>
+    <t>Batu Tangga</t>
+  </si>
+  <si>
+    <t>Tandilang</t>
+  </si>
+  <si>
+    <t>Batu Perahu</t>
+  </si>
+  <si>
+    <t>Aing Bantai</t>
+  </si>
+  <si>
+    <t>Datar Batung</t>
+  </si>
+  <si>
+    <t>Pajukungan</t>
+  </si>
+  <si>
+    <t>Bukat</t>
+  </si>
+  <si>
+    <t>Barabai Barat</t>
+  </si>
+  <si>
+    <t>Barabai Utara</t>
+  </si>
+  <si>
+    <t>Barabai Selatan</t>
+  </si>
+  <si>
+    <t>Barabai Darat</t>
+  </si>
+  <si>
+    <t>Benawa Tengah</t>
+  </si>
+  <si>
+    <t>Kayu Bawang</t>
+  </si>
+  <si>
+    <t>Awang Besar</t>
+  </si>
+  <si>
+    <t>Gambah</t>
+  </si>
+  <si>
+    <t>Mandingin</t>
+  </si>
+  <si>
+    <t>Barabai Timur</t>
+  </si>
+  <si>
+    <t>Banua Binjai</t>
+  </si>
+  <si>
+    <t>Banua Budi</t>
+  </si>
+  <si>
+    <t>Babai</t>
+  </si>
+  <si>
+    <t>Banua Jingah</t>
+  </si>
+  <si>
+    <t>Bakapas</t>
+  </si>
+  <si>
+    <t>Ayuang</t>
+  </si>
+  <si>
+    <t>Panggang Marak</t>
+  </si>
+  <si>
+    <t>Mundar</t>
+  </si>
+  <si>
+    <t>Tabudarat Hilir</t>
+  </si>
+  <si>
+    <t>Mahang Baru</t>
+  </si>
+  <si>
+    <t>Jamil</t>
+  </si>
+  <si>
+    <t>Tabudarat Hulu</t>
+  </si>
+  <si>
+    <t>Pantai Hambawang Barat</t>
+  </si>
+  <si>
+    <t>Pantai Hambawang Timur</t>
+  </si>
+  <si>
+    <t>Benua Kepayang</t>
+  </si>
+  <si>
+    <t>Sungai Jaranih</t>
+  </si>
+  <si>
+    <t>Batang Bahalang</t>
+  </si>
+  <si>
+    <t>Taal</t>
+  </si>
+  <si>
+    <t>Murung Taal</t>
+  </si>
+  <si>
+    <t>Sungai Rangas</t>
+  </si>
+  <si>
+    <t>Durian Gantang</t>
+  </si>
+  <si>
+    <t>Guha</t>
+  </si>
+  <si>
+    <t>Bangkal</t>
+  </si>
+  <si>
+    <t>Taras Padang</t>
+  </si>
+  <si>
+    <t>Pahalatan</t>
+  </si>
+  <si>
+    <t>Perumahan</t>
+  </si>
+  <si>
+    <t>Kadundung</t>
+  </si>
+  <si>
+    <t>Kasarangan</t>
+  </si>
+  <si>
+    <t>Pemangkih Seberang</t>
+  </si>
+  <si>
+    <t>Tabat</t>
+  </si>
+  <si>
+    <t>Mantaas</t>
+  </si>
+  <si>
+    <t>Rantau Bujur</t>
+  </si>
+  <si>
+    <t>Binjai Pirua</t>
+  </si>
+  <si>
+    <t>Binjai Pemangkih</t>
+  </si>
+  <si>
+    <t>Tungkup</t>
+  </si>
+  <si>
+    <t>Pemangkih</t>
+  </si>
+  <si>
+    <t>Rantau Keminting</t>
+  </si>
+  <si>
+    <t>Banua Kupang</t>
+  </si>
+  <si>
+    <t>Sungai Buluh</t>
+  </si>
+  <si>
+    <t>Samhurang</t>
+  </si>
+  <si>
+    <t>Masiraan</t>
+  </si>
+  <si>
+    <t>Jaranih</t>
+  </si>
+  <si>
+    <t>Banua Hanyar</t>
+  </si>
+  <si>
+    <t>Banua Asam</t>
+  </si>
+  <si>
+    <t>Matang Ginalun</t>
+  </si>
+  <si>
+    <t>Hulu Rasau</t>
+  </si>
+  <si>
+    <t>Banua Supanggal</t>
+  </si>
+  <si>
+    <t>Mahang Putat</t>
+  </si>
+  <si>
+    <t>Mahang Sei Hanyar</t>
+  </si>
+  <si>
+    <t>Mahang Matang Landung</t>
+  </si>
+  <si>
+    <t>Buluan</t>
+  </si>
+  <si>
+    <t>Pandawan</t>
+  </si>
+  <si>
+    <t>Banua Batung</t>
+  </si>
+  <si>
+    <t>Jatuh</t>
+  </si>
+  <si>
+    <t>Hilir Banua</t>
+  </si>
+  <si>
+    <t>Kambat Selatan</t>
+  </si>
+  <si>
+    <t>Walatung</t>
+  </si>
+  <si>
+    <t>Kayu Rabah</t>
+  </si>
+  <si>
+    <t>Setiap</t>
+  </si>
+  <si>
+    <t>Kambat Utara</t>
+  </si>
+  <si>
+    <t>Palajau</t>
+  </si>
+  <si>
+    <t>Sumanggi</t>
+  </si>
+  <si>
+    <t>Ilung Pasar Lama</t>
+  </si>
+  <si>
+    <t>Dangu</t>
+  </si>
+  <si>
+    <t>Hapingin</t>
+  </si>
+  <si>
+    <t>Ilung</t>
+  </si>
+  <si>
+    <t>Ilung Tengah</t>
+  </si>
+  <si>
+    <t>Sumanggi Seberang</t>
+  </si>
+  <si>
+    <t>Awang Baru</t>
+  </si>
+  <si>
+    <t>Awang</t>
+  </si>
+  <si>
+    <t>Maringgit</t>
+  </si>
+  <si>
+    <t>Labunganak</t>
+  </si>
+  <si>
+    <t>Muara Rintis</t>
+  </si>
+  <si>
+    <t>Telang</t>
+  </si>
+  <si>
+    <t>Haur Gading</t>
+  </si>
+  <si>
+    <t>Limpasu</t>
+  </si>
+  <si>
+    <t>Kabang</t>
+  </si>
+  <si>
+    <t>Tapuk</t>
+  </si>
+  <si>
+    <t>Pauh</t>
+  </si>
+  <si>
+    <t>Hawang</t>
+  </si>
+  <si>
+    <t>Karatungan</t>
+  </si>
+  <si>
+    <t>Abung</t>
+  </si>
+  <si>
+    <t>Abung Surapati</t>
+  </si>
+  <si>
+    <t>Karau</t>
   </si>
 </sst>
 </file>
@@ -965,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30CC73D-A967-254F-837E-CA259FBCEC82}">
-  <dimension ref="A1:B182"/>
+  <dimension ref="A1:B184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,1450 +993,1466 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>6307000</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>171</v>
+        <v>6372000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>6307010</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>172</v>
+        <v>6371000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>6307020</v>
+        <v>6307000</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>173</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6307030</v>
+        <v>6307010</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>6307040</v>
+        <v>6307020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6307041</v>
+        <v>6307030</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>176</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6307050</v>
+        <v>6307040</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>6307060</v>
+        <v>6307041</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6307070</v>
+        <v>6307050</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>179</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>6307080</v>
+        <v>6307060</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>6307090</v>
+        <v>6307070</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>6307091</v>
+        <v>6307080</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>6307010001</v>
+        <v>6307090</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>6307010003</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
+        <v>6307091</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>6307010004</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
+        <v>6307010001</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>6307010005</v>
+        <v>6307010003</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>6307010007</v>
+        <v>6307010004</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>6307010009</v>
+        <v>6307010005</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>6307010012</v>
+        <v>6307010007</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>6307010014</v>
+        <v>6307010009</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>6307010015</v>
+        <v>6307010012</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6307010016</v>
+        <v>6307010014</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>6307010019</v>
+        <v>6307010015</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>6307010021</v>
+        <v>6307010016</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>6307010022</v>
+        <v>6307010019</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>6307010024</v>
+        <v>6307010021</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6307010028</v>
+        <v>6307010022</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>6307010030</v>
+        <v>6307010024</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>6307010032</v>
+        <v>6307010028</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>6307020005</v>
+        <v>6307010030</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>6307020009</v>
+        <v>6307010032</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>6307020010</v>
+        <v>6307020005</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>6307020011</v>
+        <v>6307020009</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>6307020013</v>
+        <v>6307020010</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>6307020015</v>
+        <v>6307020011</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>6307020017</v>
+        <v>6307020013</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>6307020018</v>
+        <v>6307020015</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>6307020020</v>
+        <v>6307020017</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>6307020024</v>
+        <v>6307020018</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>6307020026</v>
+        <v>6307020020</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>6307020028</v>
+        <v>6307020024</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>6307020029</v>
+        <v>6307020026</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>6307020030</v>
+        <v>6307020028</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>6307030002</v>
+        <v>6307020029</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>6307030003</v>
+        <v>6307020030</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>6307030007</v>
+        <v>6307030002</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>6307030008</v>
+        <v>6307030003</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>6307030009</v>
+        <v>6307030007</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>6307030010</v>
+        <v>6307030008</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>6307030012</v>
+        <v>6307030009</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>6307030017</v>
+        <v>6307030010</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>6307030018</v>
+        <v>6307030012</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>6307030020</v>
+        <v>6307030017</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>6307030021</v>
+        <v>6307030018</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>6307030022</v>
+        <v>6307030020</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>6307040018</v>
+        <v>6307030021</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>6307040021</v>
+        <v>6307030022</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>6307040024</v>
+        <v>6307040018</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>6307040026</v>
+        <v>6307040021</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>6307040028</v>
+        <v>6307040024</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>6307040029</v>
+        <v>6307040026</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>6307040030</v>
+        <v>6307040028</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>6307040031</v>
+        <v>6307040029</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>6307040032</v>
+        <v>6307040030</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>6307040034</v>
+        <v>6307040031</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>6307040035</v>
+        <v>6307040032</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>6307040037</v>
+        <v>6307040034</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>6307040038</v>
+        <v>6307040035</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>6307040040</v>
+        <v>6307040037</v>
       </c>
       <c r="B70" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>6307040043</v>
+        <v>6307040038</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>6307040047</v>
+        <v>6307040040</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>6307040049</v>
+        <v>6307040043</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>6307040052</v>
+        <v>6307040047</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>6307040053</v>
+        <v>6307040049</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>6307041001</v>
+        <v>6307040052</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>6307041002</v>
+        <v>6307040053</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>6307041003</v>
+        <v>6307041001</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>6307041004</v>
+        <v>6307041002</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>6307041005</v>
+        <v>6307041003</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>6307041006</v>
+        <v>6307041004</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>6307041007</v>
+        <v>6307041005</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>6307041008</v>
+        <v>6307041006</v>
       </c>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>6307041009</v>
+        <v>6307041007</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>6307041010</v>
+        <v>6307041008</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>6307041011</v>
+        <v>6307041009</v>
       </c>
       <c r="B86" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>6307050002</v>
+        <v>6307041010</v>
       </c>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>6307050004</v>
+        <v>6307041011</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>6307050005</v>
+        <v>6307050002</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>6307050006</v>
+        <v>6307050004</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>6307050007</v>
+        <v>6307050005</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>6307050008</v>
+        <v>6307050006</v>
       </c>
       <c r="B92" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>6307050009</v>
+        <v>6307050007</v>
       </c>
       <c r="B93" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>6307050010</v>
+        <v>6307050008</v>
       </c>
       <c r="B94" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>6307050013</v>
+        <v>6307050009</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>6307050014</v>
+        <v>6307050010</v>
       </c>
       <c r="B96" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>6307050016</v>
+        <v>6307050013</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>6307050018</v>
+        <v>6307050014</v>
       </c>
       <c r="B98" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>6307050020</v>
+        <v>6307050016</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>6307050021</v>
+        <v>6307050018</v>
       </c>
       <c r="B100" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>6307050023</v>
+        <v>6307050020</v>
       </c>
       <c r="B101" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>6307050025</v>
+        <v>6307050021</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>6307050028</v>
+        <v>6307050023</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>6307050029</v>
+        <v>6307050025</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>6307060002</v>
+        <v>6307050028</v>
       </c>
       <c r="B105" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>6307060004</v>
+        <v>6307050029</v>
       </c>
       <c r="B106" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>6307060007</v>
+        <v>6307060002</v>
       </c>
       <c r="B107" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>6307060008</v>
+        <v>6307060004</v>
       </c>
       <c r="B108" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>6307060010</v>
+        <v>6307060007</v>
       </c>
       <c r="B109" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>6307060011</v>
+        <v>6307060008</v>
       </c>
       <c r="B110" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>6307060013</v>
+        <v>6307060010</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>6307060014</v>
+        <v>6307060011</v>
       </c>
       <c r="B112" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>6307060017</v>
+        <v>6307060013</v>
       </c>
       <c r="B113" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>6307060019</v>
+        <v>6307060014</v>
       </c>
       <c r="B114" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>6307060021</v>
+        <v>6307060017</v>
       </c>
       <c r="B115" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>6307060022</v>
+        <v>6307060019</v>
       </c>
       <c r="B116" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>6307060024</v>
+        <v>6307060021</v>
       </c>
       <c r="B117" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>6307060027</v>
+        <v>6307060022</v>
       </c>
       <c r="B118" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>6307060029</v>
+        <v>6307060024</v>
       </c>
       <c r="B119" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>6307060032</v>
+        <v>6307060027</v>
       </c>
       <c r="B120" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>6307060033</v>
+        <v>6307060029</v>
       </c>
       <c r="B121" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>6307060035</v>
+        <v>6307060032</v>
       </c>
       <c r="B122" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>6307070001</v>
+        <v>6307060033</v>
       </c>
       <c r="B123" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>6307070003</v>
+        <v>6307060035</v>
       </c>
       <c r="B124" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>6307070004</v>
+        <v>6307070001</v>
       </c>
       <c r="B125" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>6307070006</v>
+        <v>6307070003</v>
       </c>
       <c r="B126" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>6307070007</v>
+        <v>6307070004</v>
       </c>
       <c r="B127" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>6307070010</v>
+        <v>6307070006</v>
       </c>
       <c r="B128" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>6307070013</v>
+        <v>6307070007</v>
       </c>
       <c r="B129" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>6307070015</v>
+        <v>6307070010</v>
       </c>
       <c r="B130" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>6307070017</v>
+        <v>6307070013</v>
       </c>
       <c r="B131" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>6307070019</v>
+        <v>6307070015</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>6307070021</v>
+        <v>6307070017</v>
       </c>
       <c r="B133" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>6307070023</v>
+        <v>6307070019</v>
       </c>
       <c r="B134" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>6307070026</v>
+        <v>6307070021</v>
       </c>
       <c r="B135" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>6307070027</v>
+        <v>6307070023</v>
       </c>
       <c r="B136" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>6307070031</v>
+        <v>6307070026</v>
       </c>
       <c r="B137" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>6307070033</v>
+        <v>6307070027</v>
       </c>
       <c r="B138" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>6307080001</v>
+        <v>6307070031</v>
       </c>
       <c r="B139" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>6307080003</v>
+        <v>6307070033</v>
       </c>
       <c r="B140" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>6307080004</v>
+        <v>6307080001</v>
       </c>
       <c r="B141" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>6307080006</v>
+        <v>6307080003</v>
       </c>
       <c r="B142" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>6307080009</v>
+        <v>6307080004</v>
       </c>
       <c r="B143" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>6307080010</v>
+        <v>6307080006</v>
       </c>
       <c r="B144" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>6307080011</v>
+        <v>6307080009</v>
       </c>
       <c r="B145" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>6307080014</v>
+        <v>6307080010</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>6307080016</v>
+        <v>6307080011</v>
       </c>
       <c r="B147" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>6307080017</v>
+        <v>6307080014</v>
       </c>
       <c r="B148" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>6307080021</v>
+        <v>6307080016</v>
       </c>
       <c r="B149" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>6307080022</v>
+        <v>6307080017</v>
       </c>
       <c r="B150" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>6307080023</v>
+        <v>6307080021</v>
       </c>
       <c r="B151" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>6307080025</v>
+        <v>6307080022</v>
       </c>
       <c r="B152" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>6307080027</v>
+        <v>6307080023</v>
       </c>
       <c r="B153" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>6307080028</v>
+        <v>6307080025</v>
       </c>
       <c r="B154" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>6307080030</v>
+        <v>6307080027</v>
       </c>
       <c r="B155" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>6307080033</v>
+        <v>6307080028</v>
       </c>
       <c r="B156" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>6307080037</v>
+        <v>6307080030</v>
       </c>
       <c r="B157" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>6307080039</v>
+        <v>6307080033</v>
       </c>
       <c r="B158" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>6307080042</v>
+        <v>6307080037</v>
       </c>
       <c r="B159" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>6307090003</v>
+        <v>6307080039</v>
       </c>
       <c r="B160" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>6307090007</v>
+        <v>6307080042</v>
       </c>
       <c r="B161" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162">
-        <v>6307090009</v>
+        <v>6307090003</v>
       </c>
       <c r="B162" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>6307090011</v>
+        <v>6307090007</v>
       </c>
       <c r="B163" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>6307090012</v>
+        <v>6307090009</v>
       </c>
       <c r="B164" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>6307090013</v>
+        <v>6307090011</v>
       </c>
       <c r="B165" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>6307090014</v>
+        <v>6307090012</v>
       </c>
       <c r="B166" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>6307090016</v>
+        <v>6307090013</v>
       </c>
       <c r="B167" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168">
-        <v>6307090018</v>
+        <v>6307090014</v>
       </c>
       <c r="B168" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>6307090019</v>
+        <v>6307090016</v>
       </c>
       <c r="B169" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170">
-        <v>6307090020</v>
+        <v>6307090018</v>
       </c>
       <c r="B170" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171">
-        <v>6307090033</v>
+        <v>6307090019</v>
       </c>
       <c r="B171" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172">
-        <v>6307090035</v>
+        <v>6307090020</v>
       </c>
       <c r="B172" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173">
-        <v>6307090036</v>
+        <v>6307090033</v>
       </c>
       <c r="B173" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174">
-        <v>6307091001</v>
+        <v>6307090035</v>
       </c>
       <c r="B174" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175">
-        <v>6307091002</v>
+        <v>6307090036</v>
       </c>
       <c r="B175" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176">
-        <v>6307091003</v>
+        <v>6307091001</v>
       </c>
       <c r="B176" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177">
-        <v>6307091004</v>
+        <v>6307091002</v>
       </c>
       <c r="B177" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178">
-        <v>6307091005</v>
+        <v>6307091003</v>
       </c>
       <c r="B178" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179">
-        <v>6307091006</v>
+        <v>6307091004</v>
       </c>
       <c r="B179" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180">
-        <v>6307091007</v>
+        <v>6307091005</v>
       </c>
       <c r="B180" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>6307091008</v>
+        <v>6307091006</v>
       </c>
       <c r="B181" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182">
+        <v>6307091007</v>
+      </c>
+      <c r="B182" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>6307091008</v>
+      </c>
+      <c r="B183" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
         <v>6307091009</v>
       </c>
-      <c r="B182" t="s">
-        <v>170</v>
+      <c r="B184" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>